<commit_message>
added a FileLoadTest class for our files. Made the clueBoard into a .csv file for import.
</commit_message>
<xml_diff>
--- a/clueBoard.xlsx
+++ b/clueBoard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bane/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bane/school/semesters/fall_2016/softEng/workspace/ClueGameBSMW/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+      <selection activeCell="A23" sqref="A23:W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,9 +511,6 @@
       <c r="W1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X1">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -585,9 +582,6 @@
       <c r="W2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -659,9 +653,6 @@
       <c r="W3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -733,9 +724,6 @@
       <c r="W4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -807,9 +795,6 @@
       <c r="W5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -881,9 +866,6 @@
       <c r="W6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -955,9 +937,6 @@
       <c r="W7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="X7">
-        <v>6</v>
-      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1029,9 +1008,6 @@
       <c r="W8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X8">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1103,9 +1079,6 @@
       <c r="W9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X9">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -1177,9 +1150,6 @@
       <c r="W10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X10">
-        <v>9</v>
-      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1251,9 +1221,6 @@
       <c r="W11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X11">
-        <v>10</v>
-      </c>
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -1326,9 +1293,6 @@
       <c r="W12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X12">
-        <v>11</v>
-      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -1400,9 +1364,6 @@
       <c r="W13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="X13">
-        <v>12</v>
-      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1474,9 +1435,6 @@
       <c r="W14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="X14">
-        <v>13</v>
-      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1548,9 +1506,6 @@
       <c r="W15" t="s">
         <v>10</v>
       </c>
-      <c r="X15">
-        <v>14</v>
-      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1622,11 +1577,8 @@
       <c r="W16" t="s">
         <v>10</v>
       </c>
-      <c r="X16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
@@ -1696,11 +1648,8 @@
       <c r="W17" t="s">
         <v>10</v>
       </c>
-      <c r="X17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -1770,11 +1719,8 @@
       <c r="W18" t="s">
         <v>10</v>
       </c>
-      <c r="X18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1844,11 +1790,8 @@
       <c r="W19" t="s">
         <v>10</v>
       </c>
-      <c r="X19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1918,11 +1861,8 @@
       <c r="W20" t="s">
         <v>10</v>
       </c>
-      <c r="X20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1992,11 +1932,8 @@
       <c r="W21" t="s">
         <v>10</v>
       </c>
-      <c r="X21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2065,80 +2002,6 @@
       </c>
       <c r="W22" t="s">
         <v>10</v>
-      </c>
-      <c r="X22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="G23">
-        <v>6</v>
-      </c>
-      <c r="H23">
-        <v>7</v>
-      </c>
-      <c r="I23">
-        <v>8</v>
-      </c>
-      <c r="J23">
-        <v>9</v>
-      </c>
-      <c r="K23">
-        <v>10</v>
-      </c>
-      <c r="L23">
-        <v>11</v>
-      </c>
-      <c r="M23">
-        <v>12</v>
-      </c>
-      <c r="N23">
-        <v>13</v>
-      </c>
-      <c r="O23">
-        <v>14</v>
-      </c>
-      <c r="P23">
-        <v>15</v>
-      </c>
-      <c r="Q23">
-        <v>16</v>
-      </c>
-      <c r="R23">
-        <v>17</v>
-      </c>
-      <c r="S23">
-        <v>18</v>
-      </c>
-      <c r="T23">
-        <v>19</v>
-      </c>
-      <c r="U23">
-        <v>20</v>
-      </c>
-      <c r="V23">
-        <v>21</v>
-      </c>
-      <c r="W23">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemeted test methods and hardcoded the correct results for the FileLoadTests class
</commit_message>
<xml_diff>
--- a/clueBoard.xlsx
+++ b/clueBoard.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27680" windowHeight="18360" tabRatio="500"/>
+    <workbookView xWindow="18820" yWindow="1840" windowWidth="27680" windowHeight="18360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:W23"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,6 +511,9 @@
       <c r="W1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -582,6 +585,9 @@
       <c r="W2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -653,6 +659,9 @@
       <c r="W3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -724,6 +733,9 @@
       <c r="W4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -795,6 +807,9 @@
       <c r="W5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -866,6 +881,9 @@
       <c r="W6" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -937,6 +955,9 @@
       <c r="W7" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1008,6 +1029,9 @@
       <c r="W8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="X8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1079,6 +1103,9 @@
       <c r="W9" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="X9">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -1150,6 +1177,9 @@
       <c r="W10" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="X10">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1221,6 +1251,9 @@
       <c r="W11" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="X11">
+        <v>10</v>
+      </c>
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
@@ -1293,6 +1326,9 @@
       <c r="W12" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="X12">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -1364,6 +1400,9 @@
       <c r="W13" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="X13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1435,6 +1474,9 @@
       <c r="W14" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="X14">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1506,6 +1548,9 @@
       <c r="W15" t="s">
         <v>10</v>
       </c>
+      <c r="X15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1577,8 +1622,11 @@
       <c r="W16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
@@ -1648,8 +1696,11 @@
       <c r="W17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -1719,8 +1770,11 @@
       <c r="W18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1790,8 +1844,11 @@
       <c r="W19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1861,8 +1918,11 @@
       <c r="W20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1932,8 +1992,11 @@
       <c r="W21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2002,6 +2065,80 @@
       </c>
       <c r="W22" t="s">
         <v>10</v>
+      </c>
+      <c r="X22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23">
+        <v>11</v>
+      </c>
+      <c r="M23">
+        <v>12</v>
+      </c>
+      <c r="N23">
+        <v>13</v>
+      </c>
+      <c r="O23">
+        <v>14</v>
+      </c>
+      <c r="P23">
+        <v>15</v>
+      </c>
+      <c r="Q23">
+        <v>16</v>
+      </c>
+      <c r="R23">
+        <v>17</v>
+      </c>
+      <c r="S23">
+        <v>18</v>
+      </c>
+      <c r="T23">
+        <v>19</v>
+      </c>
+      <c r="U23">
+        <v>20</v>
+      </c>
+      <c r="V23">
+        <v>21</v>
+      </c>
+      <c r="W23">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in stub for CalcAdjacencies and completed adjacency tests, as well as color coded the Excel appropriately
</commit_message>
<xml_diff>
--- a/clueBoard.xlsx
+++ b/clueBoard.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bane/school/semesters/fall_2016/softEng/workspace/ClueGameBSMW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Software Engineering\ClueGameBSMW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="760" windowWidth="20060" windowHeight="18340" tabRatio="500"/>
+    <workbookView xWindow="4080" yWindow="765" windowWidth="20055" windowHeight="18345" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="24">
   <si>
     <t>W</t>
   </si>
@@ -90,13 +87,22 @@
   </si>
   <si>
     <t>BL</t>
+  </si>
+  <si>
+    <t>Number of doors: 16</t>
+  </si>
+  <si>
+    <t>Orange: adjacency tests for walkways</t>
+  </si>
+  <si>
+    <t>Black: adjacency tests for cells inside rooms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,8 +116,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,7 +151,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,14 +192,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,6 +214,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -440,15 +485,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -458,7 +503,7 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -522,8 +567,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -596,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -624,7 +669,7 @@
       <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -660,7 +705,7 @@
       <c r="U3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="W3" s="2" t="s">
@@ -670,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -744,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -818,7 +863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -849,7 +894,7 @@
       <c r="J6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="10" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -892,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -938,7 +983,7 @@
       <c r="O7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="Q7" s="3" t="s">
@@ -966,7 +1011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
@@ -1130,10 +1175,10 @@
       <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="10" t="s">
         <v>0</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1166,7 +1211,7 @@
       <c r="Q10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="R10" s="10" t="s">
         <v>0</v>
       </c>
       <c r="S10" s="5" t="s">
@@ -1188,7 +1233,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1263,7 +1308,7 @@
       </c>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1324,7 @@
       <c r="E12" t="s">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1337,7 +1382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
@@ -1411,8 +1456,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1478,14 +1523,14 @@
       <c r="V14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W14" s="3" t="s">
+      <c r="W14" s="7" t="s">
         <v>0</v>
       </c>
       <c r="X14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1540,7 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
@@ -1507,7 +1552,7 @@
       <c r="G15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -1559,7 +1604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -1578,7 +1623,7 @@
       <c r="F16" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -1633,8 +1678,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B17" t="s">
@@ -1673,7 +1718,7 @@
       <c r="M17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N17" s="7" t="s">
         <v>0</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -1707,7 +1752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
@@ -1781,7 +1826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1855,7 +1900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1929,7 +1974,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2003,7 +2048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2043,7 +2088,7 @@
       <c r="M22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="N22" s="7" t="s">
         <v>0</v>
       </c>
       <c r="O22" s="3" t="s">
@@ -2077,7 +2122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2148,7 +2193,23 @@
         <v>22</v>
       </c>
     </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated spreadsheet to reflect the adjancecny tests.
</commit_message>
<xml_diff>
--- a/clueBoard.xlsx
+++ b/clueBoard.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max\Documents\Software Engineering\ClueGameBSMW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bane/school/semesters/fall_2016/softEng/workspace/ClueGameBSMW/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="765" windowWidth="20055" windowHeight="18345" tabRatio="500"/>
+    <workbookView xWindow="4080" yWindow="760" windowWidth="20060" windowHeight="18340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="27">
   <si>
     <t>W</t>
   </si>
@@ -96,6 +99,15 @@
   </si>
   <si>
     <t>Black: adjacency tests for cells inside rooms</t>
+  </si>
+  <si>
+    <t>Purple: Tests adjancency for walkways next to a room (wall) that are not doorways</t>
+  </si>
+  <si>
+    <t>Green: Tests walkway cells next to doorway for the correct doorway direction (makes sure doors ae considered adjacent)</t>
+  </si>
+  <si>
+    <t>Brown: Test the doors to make sure they only have one cell in their adjacency lists</t>
   </si>
 </sst>
 </file>
@@ -485,13 +497,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z28"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2206,6 +2218,21 @@
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated spreadsheet to reflect target tests
</commit_message>
<xml_diff>
--- a/clueBoard.xlsx
+++ b/clueBoard.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="760" windowWidth="20060" windowHeight="18340" tabRatio="500"/>
+    <workbookView xWindow="5640" yWindow="660" windowWidth="20060" windowHeight="19520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="29">
   <si>
     <t>W</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Brown: Test the doors to make sure they only have one cell in their adjacency lists</t>
+  </si>
+  <si>
+    <t>Adjancency Tests:</t>
+  </si>
+  <si>
+    <t>Dark Blue: Target Tests</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -204,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -217,6 +229,8 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +802,7 @@
       <c r="T4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" s="13" t="s">
         <v>0</v>
       </c>
       <c r="V4" s="5" t="s">
@@ -832,7 +846,7 @@
       <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="13" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -1300,7 +1314,7 @@
       <c r="R11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S11" s="5" t="s">
+      <c r="S11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="T11" s="2" t="s">
@@ -1523,7 +1537,7 @@
       <c r="R14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="S14" s="3" t="s">
+      <c r="S14" s="13" t="s">
         <v>0</v>
       </c>
       <c r="T14" s="3" t="s">
@@ -1857,7 +1871,7 @@
       <c r="F19" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="13" t="s">
         <v>0</v>
       </c>
       <c r="H19" s="5" t="s">
@@ -2118,7 +2132,7 @@
       <c r="S22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="T22" s="3" t="s">
+      <c r="T22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="U22" s="2" t="s">
@@ -2134,74 +2148,74 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23" s="12">
+        <v>0</v>
+      </c>
+      <c r="B23" s="12">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12">
+        <v>2</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3</v>
+      </c>
+      <c r="E23" s="12">
+        <v>4</v>
+      </c>
+      <c r="F23" s="12">
         <v>5</v>
       </c>
-      <c r="G23">
-        <v>6</v>
-      </c>
-      <c r="H23">
-        <v>7</v>
-      </c>
-      <c r="I23">
-        <v>8</v>
-      </c>
-      <c r="J23">
-        <v>9</v>
-      </c>
-      <c r="K23">
-        <v>10</v>
-      </c>
-      <c r="L23">
+      <c r="G23" s="12">
+        <v>6</v>
+      </c>
+      <c r="H23" s="12">
+        <v>7</v>
+      </c>
+      <c r="I23" s="12">
+        <v>8</v>
+      </c>
+      <c r="J23" s="12">
+        <v>9</v>
+      </c>
+      <c r="K23" s="12">
+        <v>10</v>
+      </c>
+      <c r="L23" s="12">
         <v>11</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="12">
         <v>12</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="12">
         <v>13</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="12">
         <v>14</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="12">
         <v>15</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="12">
         <v>16</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="12">
         <v>17</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="12">
         <v>18</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="12">
         <v>19</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="12">
         <v>20</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="12">
         <v>21</v>
       </c>
-      <c r="W23">
+      <c r="W23" s="12">
         <v>22</v>
       </c>
     </row>
@@ -2212,27 +2226,37 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>